<commit_message>
This should take care of #3, but reverses Buff2Guest and Host2Guest order.
This was necessary to find the right scaling factors. We might want to store the experiments and add them to the set in reverse order, in case we do manage to improve time between experiments due to cleaning.
</commit_message>
<xml_diff>
--- a/SAMPL4-CB7/itc/run-itc.xlsx
+++ b/SAMPL4-CB7/itc/run-itc.xlsx
@@ -764,10 +764,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>87</v>
@@ -776,10 +776,10 @@
         <v>25</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2</v>
+        <v>0.11548098638506921</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1.0156055482758117</v>
       </c>
       <c r="H5" t="s">
         <v>56</v>
@@ -796,10 +796,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>87</v>
@@ -811,7 +811,7 @@
         <v>0.11548098638506921</v>
       </c>
       <c r="G6" t="n">
-        <v>1.0156055482758117</v>
+        <v>0</v>
       </c>
       <c r="H6" t="s">
         <v>29</v>
@@ -828,10 +828,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
         <v>87</v>
@@ -840,10 +840,10 @@
         <v>25</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2</v>
+        <v>0.10566411179879161</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1.0156055482758117</v>
       </c>
       <c r="H7" t="s">
         <v>39</v>
@@ -860,10 +860,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>87</v>
@@ -875,7 +875,7 @@
         <v>0.10566411179879161</v>
       </c>
       <c r="G8" t="n">
-        <v>1.0156055482758117</v>
+        <v>0</v>
       </c>
       <c r="H8" t="s">
         <v>49</v>
@@ -892,10 +892,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
         <v>87</v>
@@ -904,10 +904,10 @@
         <v>25</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2</v>
+        <v>0.031313635851805112</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H9" t="s">
         <v>57</v>
@@ -924,10 +924,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>87</v>
@@ -939,7 +939,7 @@
         <v>0.031313635851805112</v>
       </c>
       <c r="G10" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
@@ -956,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
         <v>87</v>
@@ -968,10 +968,10 @@
         <v>25</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2</v>
+        <v>0.069448775831103718</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H11" t="s">
         <v>40</v>
@@ -988,10 +988,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>87</v>
@@ -1003,7 +1003,7 @@
         <v>0.069448775831103718</v>
       </c>
       <c r="G12" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H12" t="s">
         <v>50</v>
@@ -1020,10 +1020,10 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
         <v>87</v>
@@ -1032,10 +1032,10 @@
         <v>25</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2</v>
+        <v>0.072256232169153764</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H13" t="s">
         <v>58</v>
@@ -1052,10 +1052,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
         <v>87</v>
@@ -1067,7 +1067,7 @@
         <v>0.072256232169153764</v>
       </c>
       <c r="G14" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H14" t="s">
         <v>31</v>
@@ -1084,10 +1084,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
         <v>87</v>
@@ -1096,10 +1096,10 @@
         <v>25</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2</v>
+        <v>0.057658233950277075</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H15" t="s">
         <v>41</v>
@@ -1116,10 +1116,10 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
         <v>87</v>
@@ -1131,7 +1131,7 @@
         <v>0.057658233950277075</v>
       </c>
       <c r="G16" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H16" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Buffer to buffer titration implemented. Close #4.
</commit_message>
<xml_diff>
--- a/SAMPL4-CB7/itc/run-itc.xlsx
+++ b/SAMPL4-CB7/itc/run-itc.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
   <si>
     <t>20140630a1</t>
   </si>
@@ -47,6 +47,9 @@
     <t>20140630a18</t>
   </si>
   <si>
+    <t>20140630a19</t>
+  </si>
+  <si>
     <t>20140630a2</t>
   </si>
   <si>
@@ -173,6 +176,9 @@
     <t>Plate1, E4</t>
   </si>
   <si>
+    <t>Plate1, E5</t>
+  </si>
+  <si>
     <t>Plate1, F1</t>
   </si>
   <si>
@@ -185,6 +191,9 @@
     <t>Plate1, F4</t>
   </si>
   <si>
+    <t>Plate1, F5</t>
+  </si>
+  <si>
     <t>Plate1, G1</t>
   </si>
   <si>
@@ -225,6 +234,9 @@
   </si>
   <si>
     <t>SaveSampleDestination</t>
+  </si>
+  <si>
+    <t>buffer into buffer 1</t>
   </si>
   <si>
     <t>buffer into guest01</t>
@@ -620,7 +632,7 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -630,37 +642,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -668,16 +680,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -686,30 +698,30 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -718,30 +730,30 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -750,205 +762,205 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" t="n">
-        <v>0.11548098638506921</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1.0156055482758117</v>
+        <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" t="n">
         <v>0.11548098638506921</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1.0156055482758117</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7" t="n">
-        <v>0.10566411179879161</v>
+        <v>0.11548098638506921</v>
       </c>
       <c r="G7" t="n">
-        <v>1.0156055482758117</v>
+        <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" t="n">
         <v>0.10566411179879161</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1.0156055482758117</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F9" t="n">
-        <v>0.031313635851805112</v>
+        <v>0.10566411179879161</v>
       </c>
       <c r="G9" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F10" t="n">
         <v>0.031313635851805112</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -956,31 +968,31 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F11" t="n">
-        <v>0.069448775831103718</v>
+        <v>0.031313635851805112</v>
       </c>
       <c r="G11" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -988,31 +1000,31 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F12" t="n">
         <v>0.069448775831103718</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1020,31 +1032,31 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.069448775831103718</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" t="s">
         <v>65</v>
       </c>
-      <c r="D13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.072256232169153764</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1.0156055482758115</v>
-      </c>
-      <c r="H13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" t="s">
-        <v>62</v>
-      </c>
       <c r="K13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1052,31 +1064,31 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F14" t="n">
         <v>0.072256232169153764</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1084,31 +1096,31 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F15" t="n">
-        <v>0.057658233950277075</v>
+        <v>0.072256232169153764</v>
       </c>
       <c r="G15" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1116,31 +1128,31 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F16" t="n">
         <v>0.057658233950277075</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1148,31 +1160,31 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.057658233950277075</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K17" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1180,16 +1192,16 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1198,13 +1210,13 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1212,16 +1224,16 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1230,13 +1242,45 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K19" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new ITC scripts. See #2.
</commit_message>
<xml_diff>
--- a/SAMPL4-CB7/itc/run-itc.xlsx
+++ b/SAMPL4-CB7/itc/run-itc.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>20140630a1</t>
   </si>
@@ -86,6 +86,12 @@
     <t>Chodera Load Cell Without Cleaning Cell After.setup</t>
   </si>
   <si>
+    <t>ChoderaHostGuest.inj</t>
+  </si>
+  <si>
+    <t>ChoderaWaterWater.inj</t>
+  </si>
+  <si>
     <t>Control</t>
   </si>
   <si>
@@ -288,9 +294,6 @@
   </si>
   <si>
     <t>initial cleaning water titration</t>
-  </si>
-  <si>
-    <t>jdccaiicbs.inj</t>
   </si>
   <si>
     <t>water into water 1</t>
@@ -642,16 +645,16 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
@@ -660,19 +663,19 @@
         <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
         <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -680,16 +683,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -698,13 +701,13 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -712,16 +715,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -730,13 +733,13 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -744,16 +747,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -762,13 +765,13 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -776,16 +779,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -794,13 +797,13 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -808,16 +811,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6" t="n">
         <v>0.11548098638506921</v>
@@ -826,13 +829,13 @@
         <v>1.0156055482758117</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -840,16 +843,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F7" t="n">
         <v>0.11548098638506921</v>
@@ -858,13 +861,13 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -872,16 +875,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F8" t="n">
         <v>0.10566411179879161</v>
@@ -890,13 +893,13 @@
         <v>1.0156055482758117</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -904,16 +907,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F9" t="n">
         <v>0.10566411179879161</v>
@@ -922,13 +925,13 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -936,16 +939,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F10" t="n">
         <v>0.031313635851805112</v>
@@ -954,13 +957,13 @@
         <v>1.0156055482758115</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -968,16 +971,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F11" t="n">
         <v>0.031313635851805112</v>
@@ -986,13 +989,13 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1000,16 +1003,16 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F12" t="n">
         <v>0.069448775831103718</v>
@@ -1018,13 +1021,13 @@
         <v>1.0156055482758115</v>
       </c>
       <c r="H12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1032,16 +1035,16 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F13" t="n">
         <v>0.069448775831103718</v>
@@ -1050,13 +1053,13 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1064,16 +1067,16 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F14" t="n">
         <v>0.072256232169153764</v>
@@ -1082,13 +1085,13 @@
         <v>1.0156055482758115</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1096,16 +1099,16 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F15" t="n">
         <v>0.072256232169153764</v>
@@ -1114,13 +1117,13 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1128,16 +1131,16 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F16" t="n">
         <v>0.057658233950277075</v>
@@ -1146,13 +1149,13 @@
         <v>1.0156055482758115</v>
       </c>
       <c r="H16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1160,16 +1163,16 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F17" t="n">
         <v>0.057658233950277075</v>
@@ -1178,13 +1181,13 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1192,16 +1195,16 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1210,13 +1213,13 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1224,16 +1227,16 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1242,13 +1245,13 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1256,16 +1259,16 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1274,13 +1277,13 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Buffer into guest titrations are now performed before host into guest titrations.
</commit_message>
<xml_diff>
--- a/SAMPL4-CB7/itc/run-itc.xlsx
+++ b/SAMPL4-CB7/itc/run-itc.xlsx
@@ -811,10 +811,10 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -826,7 +826,7 @@
         <v>0.11548098638506921</v>
       </c>
       <c r="G6" t="n">
-        <v>1.0156055482758117</v>
+        <v>0</v>
       </c>
       <c r="H6" t="s">
         <v>32</v>
@@ -843,10 +843,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -858,7 +858,7 @@
         <v>0.11548098638506921</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1.0156055482758117</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -875,10 +875,10 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -890,7 +890,7 @@
         <v>0.10566411179879161</v>
       </c>
       <c r="G8" t="n">
-        <v>1.0156055482758117</v>
+        <v>0</v>
       </c>
       <c r="H8" t="s">
         <v>52</v>
@@ -907,10 +907,10 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
@@ -922,7 +922,7 @@
         <v>0.10566411179879161</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1.0156055482758117</v>
       </c>
       <c r="H9" t="s">
         <v>62</v>
@@ -939,10 +939,10 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
@@ -954,7 +954,7 @@
         <v>0.031313635851805112</v>
       </c>
       <c r="G10" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -971,10 +971,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -986,7 +986,7 @@
         <v>0.031313635851805112</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H11" t="s">
         <v>43</v>
@@ -1003,10 +1003,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
@@ -1018,7 +1018,7 @@
         <v>0.069448775831103718</v>
       </c>
       <c r="G12" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H12" t="s">
         <v>53</v>
@@ -1035,10 +1035,10 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
@@ -1050,7 +1050,7 @@
         <v>0.069448775831103718</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H13" t="s">
         <v>63</v>
@@ -1067,10 +1067,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
@@ -1082,7 +1082,7 @@
         <v>0.072256232169153764</v>
       </c>
       <c r="G14" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H14" t="s">
         <v>34</v>
@@ -1099,10 +1099,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
         <v>23</v>
@@ -1114,7 +1114,7 @@
         <v>0.072256232169153764</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H15" t="s">
         <v>44</v>
@@ -1131,10 +1131,10 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
@@ -1146,7 +1146,7 @@
         <v>0.057658233950277075</v>
       </c>
       <c r="G16" t="n">
-        <v>1.0156055482758115</v>
+        <v>0</v>
       </c>
       <c r="H16" t="s">
         <v>54</v>
@@ -1163,10 +1163,10 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
@@ -1178,7 +1178,7 @@
         <v>0.057658233950277075</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1.0156055482758115</v>
       </c>
       <c r="H17" t="s">
         <v>64</v>

</xml_diff>